<commit_message>
files mostly ready to order now
</commit_message>
<xml_diff>
--- a/unoshield-v5-bom.xlsx
+++ b/unoshield-v5-bom.xlsx
@@ -5,12 +5,12 @@
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/c7896e7ab03a0275/Documents/GitHub/trashrobot4/circuitboards/unoshield/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lafel\OneDrive\Documents\GitHub\trashrobot5\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="23" documentId="8_{786209F5-C015-42DF-8439-BD069CB84789}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{A518FDC4-3733-4913-A758-A42C571A3B40}"/>
+  <xr:revisionPtr revIDLastSave="26" documentId="8_{786209F5-C015-42DF-8439-BD069CB84789}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{CB1E9C3F-9002-454E-B6F1-08FA463261DA}"/>
   <bookViews>
-    <workbookView xWindow="1853" yWindow="803" windowWidth="18337" windowHeight="12442" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="368" yWindow="368" windowWidth="18337" windowHeight="12442" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="178" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="173" uniqueCount="74">
   <si>
     <t>REFDES</t>
   </si>
@@ -111,9 +111,6 @@
     <t>DO-214AC</t>
   </si>
   <si>
-    <t>PTV09A-4030U-B203-ND</t>
-  </si>
-  <si>
     <t>10k</t>
   </si>
   <si>
@@ -144,15 +141,9 @@
     <t>RR0816P-301-D</t>
   </si>
   <si>
-    <t>20k pot</t>
-  </si>
-  <si>
     <t>R5</t>
   </si>
   <si>
-    <t>PTV09A-4030U-B203</t>
-  </si>
-  <si>
     <t>Bourns, inc</t>
   </si>
   <si>
@@ -214,9 +205,6 @@
   </si>
   <si>
     <t>1528-1074-ND</t>
-  </si>
-  <si>
-    <t>R5b</t>
   </si>
   <si>
     <t>10k pot</t>
@@ -785,8 +773,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I45"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="B26" sqref="B26"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="H11" sqref="H11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.5"/>
@@ -836,19 +824,19 @@
         <v>8</v>
       </c>
       <c r="B3" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="C3" s="4">
         <v>1</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="E3" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="F3" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="H3" s="5">
         <v>0.25</v>
@@ -951,7 +939,7 @@
       <c r="F7" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="H7">
+      <c r="H7" s="5">
         <v>0.3</v>
       </c>
     </row>
@@ -998,22 +986,22 @@
         <v>13</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C11" s="3">
         <v>3</v>
       </c>
       <c r="D11" s="4" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E11" s="3" t="s">
         <v>12</v>
       </c>
       <c r="F11" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="G11" s="10" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="H11" s="5">
         <v>2.7E-2</v>
@@ -1021,25 +1009,25 @@
     </row>
     <row r="12" spans="1:9" ht="16.899999999999999" x14ac:dyDescent="0.5">
       <c r="A12" s="8" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B12" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="C12" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="D12" s="8" t="s">
         <v>28</v>
-      </c>
-      <c r="C12" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="D12" s="8" t="s">
-        <v>29</v>
       </c>
       <c r="E12" s="9" t="s">
         <v>12</v>
       </c>
       <c r="F12" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="G12" s="10" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="H12" s="5">
         <v>2.7E-2</v>
@@ -1047,25 +1035,25 @@
     </row>
     <row r="13" spans="1:9" ht="16.899999999999999" x14ac:dyDescent="0.5">
       <c r="A13" s="8" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B13" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="C13" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="D13" s="8" t="s">
         <v>28</v>
-      </c>
-      <c r="C13" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="D13" s="8" t="s">
-        <v>29</v>
       </c>
       <c r="E13" s="9" t="s">
         <v>12</v>
       </c>
       <c r="F13" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="G13" s="10" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="H13" s="5">
         <v>2.7E-2</v>
@@ -1073,7 +1061,7 @@
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.5">
       <c r="A14" s="8" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B14">
         <v>300</v>
@@ -1082,16 +1070,16 @@
         <v>1</v>
       </c>
       <c r="D14" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="E14" t="s">
+        <v>36</v>
+      </c>
+      <c r="F14" t="s">
         <v>35</v>
       </c>
-      <c r="E14" t="s">
-        <v>37</v>
-      </c>
-      <c r="F14" t="s">
-        <v>36</v>
-      </c>
       <c r="G14" s="10" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="H14" s="5">
         <v>3.6999999999999998E-2</v>
@@ -1102,71 +1090,48 @@
     </row>
     <row r="15" spans="1:9" ht="16.899999999999999" x14ac:dyDescent="0.5">
       <c r="A15" s="8" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B15" s="9" t="s">
-        <v>38</v>
+        <v>59</v>
       </c>
       <c r="C15" s="8">
         <v>1</v>
       </c>
       <c r="D15" s="8" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="E15" t="s">
-        <v>40</v>
+        <v>61</v>
       </c>
       <c r="F15" t="s">
-        <v>27</v>
+        <v>60</v>
       </c>
       <c r="H15" s="5">
         <v>0.75</v>
       </c>
     </row>
-    <row r="16" spans="1:9" ht="16.899999999999999" x14ac:dyDescent="0.5">
-      <c r="A16" s="8" t="s">
-        <v>62</v>
-      </c>
-      <c r="B16" s="9" t="s">
-        <v>63</v>
-      </c>
-      <c r="C16" s="8">
-        <v>1</v>
-      </c>
-      <c r="D16" s="8" t="s">
-        <v>41</v>
-      </c>
-      <c r="E16" t="s">
-        <v>65</v>
-      </c>
-      <c r="F16" t="s">
-        <v>64</v>
-      </c>
-      <c r="H16" s="5">
-        <v>0.75</v>
-      </c>
-    </row>
     <row r="17" spans="1:8" ht="16.899999999999999" x14ac:dyDescent="0.5">
       <c r="A17" s="8" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="B17" s="9" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="C17">
         <v>1</v>
       </c>
       <c r="D17" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="E17" t="s">
+        <v>42</v>
+      </c>
+      <c r="F17" t="s">
+        <v>43</v>
+      </c>
+      <c r="G17" s="10" t="s">
         <v>44</v>
-      </c>
-      <c r="E17" t="s">
-        <v>45</v>
-      </c>
-      <c r="F17" t="s">
-        <v>46</v>
-      </c>
-      <c r="G17" s="10" t="s">
-        <v>47</v>
       </c>
       <c r="H17" s="5">
         <v>0.51</v>
@@ -1174,22 +1139,22 @@
     </row>
     <row r="19" spans="1:8" ht="16.899999999999999" x14ac:dyDescent="0.5">
       <c r="A19" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="B19" s="3" t="s">
         <v>48</v>
-      </c>
-      <c r="B19" s="3" t="s">
-        <v>51</v>
       </c>
       <c r="C19" s="3">
         <v>2</v>
       </c>
       <c r="D19" s="3" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="E19" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="F19" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="G19" s="9" t="s">
         <v>9</v>
@@ -1200,20 +1165,20 @@
     </row>
     <row r="20" spans="1:8" ht="16.899999999999999" x14ac:dyDescent="0.5">
       <c r="A20" s="4" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="B20" s="4" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="C20" s="4"/>
       <c r="D20" s="9" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="E20" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="F20" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="G20" s="9" t="s">
         <v>9</v>
@@ -1224,22 +1189,22 @@
     </row>
     <row r="21" spans="1:8" ht="16.899999999999999" x14ac:dyDescent="0.5">
       <c r="A21" s="8" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="B21" s="9" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="C21">
         <v>1</v>
       </c>
       <c r="D21" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="E21" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="F21" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="H21" s="5">
         <v>3.54</v>
@@ -1255,19 +1220,19 @@
         <v>14</v>
       </c>
       <c r="B23" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="C23">
         <v>1</v>
       </c>
       <c r="D23" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="E23" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="F23" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="H23" s="5">
         <v>0.68</v>
@@ -1275,10 +1240,10 @@
     </row>
     <row r="24" spans="1:8" ht="16.899999999999999" x14ac:dyDescent="0.5">
       <c r="A24" s="3" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="C24" s="3" t="s">
         <v>9</v>
@@ -1298,10 +1263,10 @@
     </row>
     <row r="25" spans="1:8" ht="16.899999999999999" x14ac:dyDescent="0.5">
       <c r="A25" s="3" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="C25" s="3" t="s">
         <v>9</v>
@@ -1321,22 +1286,22 @@
     </row>
     <row r="26" spans="1:8" ht="16.899999999999999" x14ac:dyDescent="0.5">
       <c r="A26" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="B26" s="9" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="C26">
         <v>1</v>
       </c>
       <c r="D26" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="E26">
         <v>85</v>
       </c>
       <c r="F26" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="H26" s="5">
         <v>1.95</v>
@@ -1348,12 +1313,12 @@
       </c>
       <c r="H28" s="7">
         <f>SUM(H3:H26)</f>
-        <v>10.103999999999999</v>
+        <v>9.3539999999999992</v>
       </c>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.5">
       <c r="A30" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
     </row>
     <row r="35" spans="1:8" ht="16.899999999999999" x14ac:dyDescent="0.5">

</xml_diff>